<commit_message>
Tidied up papply error messages - ff object is not supported.
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/sprint@124 edb9625f-4e0d-4859-8d74-9fd3b1da38cb

Former-commit-id: aaa58c158dc3c19cf7fdffc1654d15442af17458
</commit_message>
<xml_diff>
--- a/branches/pStringDist/test_suite/pStringDistTestResults.xlsx
+++ b/branches/pStringDist/test_suite/pStringDistTestResults.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23206"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="7000" yWindow="0" windowWidth="21500" windowHeight="11780" tabRatio="500"/>
+    <workbookView xWindow="3740" yWindow="0" windowWidth="23060" windowHeight="22540" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="hector 8 cores on 2 nodes" sheetId="1" r:id="rId1"/>
+    <sheet name="hector 8 cores on 8 nodes" sheetId="3" r:id="rId2"/>
+    <sheet name="stringDistMatrix" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="38">
   <si>
     <t>rows</t>
   </si>
@@ -84,20 +86,62 @@
     <t>-</t>
   </si>
   <si>
-    <t>killed</t>
-  </si>
-  <si>
     <t>Terminated</t>
   </si>
   <si>
     <t>Error: cannot allocate vector of size 15.1 Gb</t>
+  </si>
+  <si>
+    <t>length &gt; .Machine$integer.max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Error in if (length &lt; 0 || length &gt; .Machine$integer.max) stop("length must be between 1 and .Machine$integer.max") : </t>
+  </si>
+  <si>
+    <t xml:space="preserve">  missing value where TRUE/FALSE needed</t>
+  </si>
+  <si>
+    <t>16G</t>
+  </si>
+  <si>
+    <t>stringdistmatrix</t>
+  </si>
+  <si>
+    <t>4 cores on mac</t>
+  </si>
+  <si>
+    <t>serial on mac</t>
+  </si>
+  <si>
+    <t>segfault 'memory not mapped'</t>
+  </si>
+  <si>
+    <t>pstringdist on mac</t>
+  </si>
+  <si>
+    <t>segfault. 'memory not mapped'</t>
+  </si>
+  <si>
+    <t>Error in ff</t>
+  </si>
+  <si>
+    <t>out of memory</t>
+  </si>
+  <si>
+    <t>217 (on 16 cores and 16 nodes)</t>
+  </si>
+  <si>
+    <t>(1 p on mac)</t>
+  </si>
+  <si>
+    <t>(4 p on mac)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -121,6 +165,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Courier"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -139,17 +188,34 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="11">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -594,12 +660,6 @@
       <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="D9">
-        <v>0.23</v>
-      </c>
-      <c r="E9">
-        <v>0.221</v>
-      </c>
       <c r="G9">
         <v>11000</v>
       </c>
@@ -626,12 +686,6 @@
       <c r="C10" t="s">
         <v>10</v>
       </c>
-      <c r="D10">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.32100000000000001</v>
-      </c>
       <c r="G10">
         <v>22000</v>
       </c>
@@ -658,12 +712,6 @@
       <c r="C11" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
-        <v>0.374</v>
-      </c>
-      <c r="E11">
-        <v>0.435</v>
-      </c>
       <c r="G11">
         <v>35000</v>
       </c>
@@ -688,10 +736,10 @@
         <v>320</v>
       </c>
       <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
         <v>22</v>
-      </c>
-      <c r="E12" t="s">
-        <v>23</v>
       </c>
       <c r="G12">
         <v>45000</v>
@@ -720,7 +768,7 @@
         <v>20</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G13">
         <v>50000</v>
@@ -732,7 +780,7 @@
         <v>20</v>
       </c>
       <c r="J13" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K13">
         <v>808.25199999999995</v>
@@ -747,6 +795,362 @@
       </c>
       <c r="K14">
         <v>986.01499999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:K9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="3" max="3" width="16.5" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" customWidth="1"/>
+    <col min="9" max="9" width="15.83203125" customWidth="1"/>
+    <col min="10" max="10" width="13.83203125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4">
+        <v>11000</v>
+      </c>
+      <c r="B4">
+        <v>320</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4">
+        <v>41</v>
+      </c>
+      <c r="E4">
+        <v>50</v>
+      </c>
+      <c r="G4">
+        <v>11000</v>
+      </c>
+      <c r="H4">
+        <v>100</v>
+      </c>
+      <c r="I4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4">
+        <v>4.6669999999999998</v>
+      </c>
+      <c r="K4">
+        <v>36.023000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>22000</v>
+      </c>
+      <c r="B5">
+        <v>320</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>98</v>
+      </c>
+      <c r="E5">
+        <v>206</v>
+      </c>
+      <c r="G5">
+        <v>22000</v>
+      </c>
+      <c r="H5">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5">
+        <v>24.600999999999999</v>
+      </c>
+      <c r="K5">
+        <v>144.876</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6">
+        <v>35000</v>
+      </c>
+      <c r="B6">
+        <v>320</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>231</v>
+      </c>
+      <c r="E6">
+        <v>529</v>
+      </c>
+      <c r="G6">
+        <v>35000</v>
+      </c>
+      <c r="H6">
+        <v>100</v>
+      </c>
+      <c r="I6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J6">
+        <v>63.904000000000003</v>
+      </c>
+      <c r="K6">
+        <v>376.12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>45000</v>
+      </c>
+      <c r="B7">
+        <v>320</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7">
+        <v>886</v>
+      </c>
+      <c r="G7">
+        <v>45000</v>
+      </c>
+      <c r="H7">
+        <v>100</v>
+      </c>
+      <c r="I7" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7">
+        <v>96.375</v>
+      </c>
+      <c r="K7">
+        <v>643.91600000000005</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8">
+        <v>50000</v>
+      </c>
+      <c r="B8">
+        <v>320</v>
+      </c>
+      <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>50000</v>
+      </c>
+      <c r="H8">
+        <v>100</v>
+      </c>
+      <c r="I8" t="s">
+        <v>20</v>
+      </c>
+      <c r="J8" t="s">
+        <v>24</v>
+      </c>
+      <c r="K8">
+        <v>808.25199999999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="G9">
+        <v>55000</v>
+      </c>
+      <c r="H9">
+        <v>100</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K9">
+        <v>986.01499999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:H8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="6" max="6" width="15.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:8">
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
+      <c r="B5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8">
+      <c r="B6">
+        <v>20000</v>
+      </c>
+      <c r="C6">
+        <v>100</v>
+      </c>
+      <c r="E6">
+        <v>260</v>
+      </c>
+      <c r="F6">
+        <v>194.2</v>
+      </c>
+      <c r="G6">
+        <v>61</v>
+      </c>
+      <c r="H6">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8">
+      <c r="B7">
+        <v>46300</v>
+      </c>
+      <c r="C7">
+        <v>100</v>
+      </c>
+      <c r="E7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7">
+        <v>412</v>
+      </c>
+      <c r="H7">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8">
+      <c r="B8">
+        <v>46500</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>